<commit_message>
add data for tests
</commit_message>
<xml_diff>
--- a/examples/data/petr_options_chain_3.xlsx
+++ b/examples/data/petr_options_chain_3.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.hun\Documents\repos\option_monitor2\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE22980C-02FF-4805-93F2-D7166E82DF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E833BC51-F83C-42D8-B5C5-7C435D4C089F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{5828EF37-8FFC-474E-B380-CED8276F2316}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{5828EF37-8FFC-474E-B380-CED8276F2316}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6223,8 +6224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB6F38C-C06D-4011-9266-3D021F228CA4}">
   <dimension ref="A1:T1925"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H222" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A1887" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1901" sqref="L1901"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>